<commit_message>
Men Page Gmail Login
</commit_message>
<xml_diff>
--- a/resources/test_data/test_data.xlsx
+++ b/resources/test_data/test_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Browser</t>
   </si>
@@ -58,16 +58,36 @@
   </si>
   <si>
     <t>Shah rukh</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>charmproject17@gmail.com</t>
+  </si>
+  <si>
+    <t>Charm@1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,14 +116,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -499,7 +522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -522,12 +545,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>